<commit_message>
coragem, o cao covarde
</commit_message>
<xml_diff>
--- a/6.5 Cronograma.xlsx
+++ b/6.5 Cronograma.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="23895" windowHeight="9975"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="20730" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="84">
   <si>
     <t>Etapas</t>
   </si>
@@ -60,9 +60,6 @@
     <t>d) Requisitos do sistema</t>
   </si>
   <si>
-    <t>1.1.2 Viabilidade</t>
-  </si>
-  <si>
     <t>b) Entrevista com o analista de negócios</t>
   </si>
   <si>
@@ -150,18 +147,9 @@
     <t>b) Assinar termo de encerramento</t>
   </si>
   <si>
-    <t>1.1.1.3 Definição de Custos</t>
-  </si>
-  <si>
     <t>1.1.1.4 Criar Documento de Visão</t>
   </si>
   <si>
-    <t>1.1.2.1 Levantamento das Regras de Negócio</t>
-  </si>
-  <si>
-    <t>1.1.2.2 Identificação de Possíveis Riscos</t>
-  </si>
-  <si>
     <t>c) Adequação aos fatores culturais</t>
   </si>
   <si>
@@ -216,9 +204,6 @@
     <t>1.5.1 Termo de Encerramento</t>
   </si>
   <si>
-    <t>1.1 Iniciação e Planejamento</t>
-  </si>
-  <si>
     <t>1.1.1 Concepção</t>
   </si>
   <si>
@@ -234,9 +219,6 @@
     <t>c)Entrevista com o analista de negócios</t>
   </si>
   <si>
-    <t>1.1.1.2 Identificação dos Stakeholders</t>
-  </si>
-  <si>
     <t>a)Entrevista com o cliente</t>
   </si>
   <si>
@@ -265,13 +247,34 @@
   </si>
   <si>
     <t>Atividade do Projeto</t>
+  </si>
+  <si>
+    <t>1.1 Iniciação</t>
+  </si>
+  <si>
+    <t>1.1.1.2 Identificar dos Stakeholders</t>
+  </si>
+  <si>
+    <t>1.1.1.3 Desenvolver termo de abertura</t>
+  </si>
+  <si>
+    <t>1.2 Planejamento</t>
+  </si>
+  <si>
+    <t>1.2.1 Viabilidade</t>
+  </si>
+  <si>
+    <t>1.2.1.1 Levantamento das Regras de Negócio</t>
+  </si>
+  <si>
+    <t>1.2.1.2 Identificação de Possíveis Riscos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -408,12 +411,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -423,7 +420,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -437,6 +443,11 @@
       <color rgb="FFFBA203"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -515,6 +526,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -549,6 +561,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -724,181 +737,185 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56.28515625" customWidth="1"/>
     <col min="2" max="25" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
+    <row r="1" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="8"/>
-      <c r="C1" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="10"/>
-    </row>
-    <row r="2" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B2" s="11"/>
-      <c r="C2" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B3" s="12"/>
-      <c r="C3" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B4" s="13"/>
-      <c r="C4" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:25" ht="16.5" thickTop="1" thickBot="1"/>
-    <row r="6" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A6" s="14" t="s">
+      <c r="C1" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="9"/>
+      <c r="C2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="10"/>
+      <c r="C3" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="11"/>
+      <c r="C4" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15" t="s">
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15" t="s">
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15" t="s">
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15" t="s">
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-    </row>
-    <row r="7" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A7" s="14" t="s">
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+    </row>
+    <row r="7" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="13">
         <v>1</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="13">
         <v>2</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="13">
         <v>3</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="13">
         <v>4</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="13">
         <v>1</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="13">
         <v>2</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="13">
         <v>3</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="13">
         <v>4</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="13">
         <v>1</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="13">
         <v>2</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="13">
         <v>3</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="13">
         <v>4</v>
       </c>
-      <c r="N7" s="16">
+      <c r="N7" s="13">
         <v>1</v>
       </c>
-      <c r="O7" s="16">
+      <c r="O7" s="13">
         <v>2</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="13">
         <v>3</v>
       </c>
-      <c r="Q7" s="16">
+      <c r="Q7" s="13">
         <v>4</v>
       </c>
-      <c r="R7" s="16">
+      <c r="R7" s="13">
         <v>1</v>
       </c>
-      <c r="S7" s="16">
+      <c r="S7" s="13">
         <v>2</v>
       </c>
-      <c r="T7" s="16">
+      <c r="T7" s="13">
         <v>3</v>
       </c>
-      <c r="U7" s="16">
+      <c r="U7" s="13">
         <v>4</v>
       </c>
-      <c r="V7" s="16">
+      <c r="V7" s="13">
         <v>1</v>
       </c>
-      <c r="W7" s="16">
+      <c r="W7" s="13">
         <v>2</v>
       </c>
-      <c r="X7" s="16">
+      <c r="X7" s="13">
         <v>3</v>
       </c>
-      <c r="Y7" s="16">
+      <c r="Y7" s="13">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15.75" thickTop="1">
+    <row r="8" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -914,9 +931,9 @@
       <c r="M8" s="4"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -926,112 +943,112 @@
       <c r="G9" s="1"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:10" s="2" customFormat="1"/>
-    <row r="21" spans="1:10">
+    <row r="20" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:10" s="2" customFormat="1"/>
-    <row r="25" spans="1:10">
+    <row r="24" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1039,7 +1056,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1047,7 +1064,7 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1057,8 +1074,10 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="2"/>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1067,64 +1086,64 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:12" s="2" customFormat="1"/>
-    <row r="37" spans="1:12">
+    <row r="36" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J40" s="3"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1137,7 +1156,7 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1150,113 +1169,113 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J44" s="7"/>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:12" s="2" customFormat="1"/>
-    <row r="47" spans="1:12">
+    <row r="46" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="J47" s="7"/>
     </row>
-    <row r="48" spans="1:12" s="2" customFormat="1"/>
-    <row r="49" spans="1:14">
+    <row r="48" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>47</v>
+      </c>
+      <c r="K53" s="7"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>20</v>
       </c>
-      <c r="K51" s="3"/>
-    </row>
-    <row r="52" spans="1:14" s="2" customFormat="1"/>
-    <row r="53" spans="1:14">
-      <c r="A53" t="s">
-        <v>51</v>
-      </c>
-      <c r="K53" s="7"/>
-    </row>
-    <row r="54" spans="1:14">
-      <c r="A54" t="s">
-        <v>21</v>
-      </c>
       <c r="K54" s="3"/>
     </row>
-    <row r="55" spans="1:14" s="2" customFormat="1"/>
-    <row r="56" spans="1:14">
+    <row r="55" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="K56" s="2"/>
       <c r="L56" s="7"/>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>21</v>
+      </c>
+      <c r="L57" s="3"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>22</v>
       </c>
-      <c r="L57" s="3"/>
-    </row>
-    <row r="58" spans="1:14">
-      <c r="A58" t="s">
+      <c r="L58" s="3"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>23</v>
       </c>
-      <c r="L58" s="3"/>
-    </row>
-    <row r="59" spans="1:14">
-      <c r="A59" t="s">
+      <c r="L59" s="3"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>24</v>
       </c>
-      <c r="L59" s="3"/>
-    </row>
-    <row r="60" spans="1:14">
-      <c r="A60" t="s">
-        <v>25</v>
-      </c>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="1:14" s="2" customFormat="1"/>
-    <row r="62" spans="1:14">
+    <row r="61" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="L62" s="7"/>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -1272,7 +1291,7 @@
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -1288,9 +1307,9 @@
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L66" s="2"/>
       <c r="M66" s="1"/>
@@ -1298,244 +1317,244 @@
       <c r="O66" s="2"/>
       <c r="P66" s="2"/>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="L67" s="2"/>
       <c r="M67" s="7"/>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>26</v>
+      </c>
+      <c r="M68" s="3"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>27</v>
       </c>
-      <c r="M68" s="3"/>
-    </row>
-    <row r="69" spans="1:16">
-      <c r="A69" t="s">
+      <c r="M69" s="3"/>
+    </row>
+    <row r="70" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>50</v>
+      </c>
+      <c r="M71" s="7"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>28</v>
       </c>
-      <c r="M69" s="3"/>
-    </row>
-    <row r="70" spans="1:16" s="2" customFormat="1"/>
-    <row r="71" spans="1:16">
-      <c r="A71" t="s">
-        <v>54</v>
-      </c>
-      <c r="M71" s="7"/>
-    </row>
-    <row r="72" spans="1:16">
-      <c r="A72" t="s">
+      <c r="M72" s="3"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>51</v>
+      </c>
+      <c r="M73" s="3"/>
+    </row>
+    <row r="74" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>29</v>
-      </c>
-      <c r="M72" s="3"/>
-    </row>
-    <row r="73" spans="1:16">
-      <c r="A73" t="s">
-        <v>55</v>
-      </c>
-      <c r="M73" s="3"/>
-    </row>
-    <row r="74" spans="1:16" s="2" customFormat="1"/>
-    <row r="75" spans="1:16" s="2" customFormat="1"/>
-    <row r="76" spans="1:16">
-      <c r="A76" t="s">
-        <v>30</v>
       </c>
       <c r="M76" s="5"/>
       <c r="N76" s="5"/>
       <c r="O76" s="5"/>
       <c r="P76" s="5"/>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N78" s="3"/>
     </row>
-    <row r="79" spans="1:16" s="2" customFormat="1"/>
-    <row r="80" spans="1:16">
+    <row r="79" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
       <c r="P80" s="1"/>
     </row>
-    <row r="81" spans="1:19">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N81" s="3"/>
       <c r="O81" s="3"/>
       <c r="P81" s="3"/>
     </row>
-    <row r="82" spans="1:19">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="N82" s="3"/>
       <c r="O82" s="3"/>
       <c r="P82" s="3"/>
     </row>
-    <row r="83" spans="1:19" s="2" customFormat="1"/>
-    <row r="84" spans="1:19">
+    <row r="83" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="P84" s="1"/>
     </row>
-    <row r="85" spans="1:19">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>32</v>
+      </c>
+      <c r="P85" s="3"/>
+    </row>
+    <row r="86" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>33</v>
-      </c>
-      <c r="P85" s="3"/>
-    </row>
-    <row r="86" spans="1:19" s="2" customFormat="1"/>
-    <row r="87" spans="1:19" s="2" customFormat="1"/>
-    <row r="88" spans="1:19">
-      <c r="A88" t="s">
-        <v>34</v>
       </c>
       <c r="P88" s="4"/>
       <c r="Q88" s="4"/>
       <c r="R88" s="4"/>
       <c r="S88" s="4"/>
     </row>
-    <row r="89" spans="1:19">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
     </row>
-    <row r="90" spans="1:19">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>34</v>
+      </c>
+      <c r="P90" s="3"/>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>35</v>
       </c>
-      <c r="P90" s="3"/>
-    </row>
-    <row r="91" spans="1:19">
-      <c r="A91" t="s">
-        <v>36</v>
-      </c>
       <c r="Q91" s="3"/>
     </row>
-    <row r="92" spans="1:19" s="2" customFormat="1"/>
-    <row r="93" spans="1:19">
+    <row r="92" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
       <c r="S93" s="1"/>
     </row>
-    <row r="94" spans="1:19">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="Q94" s="3"/>
       <c r="R94" s="3"/>
       <c r="S94" s="3"/>
     </row>
-    <row r="95" spans="1:19" s="2" customFormat="1"/>
-    <row r="96" spans="1:19" s="2" customFormat="1"/>
-    <row r="97" spans="1:25">
+    <row r="95" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T97" s="4"/>
       <c r="U97" s="4"/>
       <c r="V97" s="4"/>
       <c r="W97" s="4"/>
     </row>
-    <row r="98" spans="1:25">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="T98" s="1"/>
       <c r="U98" s="1"/>
     </row>
-    <row r="99" spans="1:25">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S99" s="2"/>
       <c r="T99" s="3"/>
       <c r="U99" s="3"/>
     </row>
-    <row r="100" spans="1:25">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U100" s="3"/>
     </row>
-    <row r="101" spans="1:25" s="2" customFormat="1"/>
-    <row r="102" spans="1:25">
+    <row r="101" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="U102" s="2"/>
       <c r="V102" s="1"/>
       <c r="W102" s="1"/>
     </row>
-    <row r="103" spans="1:25">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V103" s="3"/>
       <c r="W103" s="3"/>
     </row>
-    <row r="104" spans="1:25" s="2" customFormat="1"/>
-    <row r="105" spans="1:25" s="2" customFormat="1"/>
-    <row r="106" spans="1:25">
+    <row r="104" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W106" s="4"/>
       <c r="X106" s="4"/>
       <c r="Y106" s="4"/>
     </row>
-    <row r="107" spans="1:25">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="W107" s="1"/>
       <c r="X107" s="1"/>
       <c r="Y107" s="1"/>
     </row>
-    <row r="108" spans="1:25">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="W108" s="3"/>
       <c r="X108" s="3"/>
     </row>
-    <row r="109" spans="1:25">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y109" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
     <mergeCell ref="J6:M6"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="R6:U6"/>
     <mergeCell ref="V6:Y6"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1543,24 +1562,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>